<commit_message>
actualizacion 17 marzo con cambio de nps icx
</commit_message>
<xml_diff>
--- a/Resultado/informe_diario_20250317.xlsx
+++ b/Resultado/informe_diario_20250317.xlsx
@@ -103,13 +103,13 @@
     <t>7.08%</t>
   </si>
   <si>
-    <t>4.80</t>
-  </si>
-  <si>
-    <t>81.96%</t>
-  </si>
-  <si>
-    <t>3,806,297,870,660</t>
+    <t>4.76</t>
+  </si>
+  <si>
+    <t>85.71%</t>
+  </si>
+  <si>
+    <t>3,809,370,551,113</t>
   </si>
   <si>
     <t>0.74%</t>
@@ -127,7 +127,7 @@
     <t>10.42%</t>
   </si>
   <si>
-    <t>4,386,681,142,852</t>
+    <t>4,388,130,730,022</t>
   </si>
   <si>
     <t>1.54%</t>
@@ -145,7 +145,7 @@
     <t>17.5%</t>
   </si>
   <si>
-    <t>8,192,979,013,512</t>
+    <t>8,197,501,281,135</t>
   </si>
 </sst>
 </file>
@@ -780,13 +780,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>10977575</v>
+        <v>10985752</v>
       </c>
       <c r="C20">
-        <v>13017559</v>
+        <v>13022348</v>
       </c>
       <c r="D20">
-        <v>23995134</v>
+        <v>24008100</v>
       </c>
     </row>
     <row r="21" spans="1:4">

</xml_diff>